<commit_message>
add Registers spreadsheet with PIT update
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koer2434\Documents\fpga\pyripherals\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\pyripherals\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE2DF48-9317-4225-87D8-771B41E9424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{19D91056-61DB-4532-939E-DE7DC2E351AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="9" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="13" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -26,11 +26,13 @@
     <sheet name="AD7961" sheetId="13" r:id="rId11"/>
     <sheet name="TMF8801" sheetId="17" r:id="rId12"/>
     <sheet name="DAC101C081" sheetId="18" r:id="rId13"/>
+    <sheet name="PIT" sheetId="19" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">I2C!$A$1:$E$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="344">
   <si>
     <t>Name</t>
   </si>
@@ -1054,6 +1056,33 @@
   </si>
   <si>
     <t>0xD</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>CNT</t>
+  </si>
+  <si>
+    <t>SLAVE</t>
+  </si>
+  <si>
+    <t>DECADE_CNTR</t>
+  </si>
+  <si>
+    <t>NO_PRESCALE</t>
+  </si>
+  <si>
+    <t>PRE_SCALR</t>
+  </si>
+  <si>
+    <t>FLAG</t>
+  </si>
+  <si>
+    <t>ENA_INT</t>
+  </si>
+  <si>
+    <t>CNT_EN</t>
   </si>
 </sst>
 </file>
@@ -1153,9 +1182,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1193,7 +1222,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1299,7 +1328,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1441,7 +1470,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1593,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CC0846-B885-4A4F-9321-B09606FEAD42}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -3709,6 +3738,248 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5D2289-DB12-4156-86D5-FCA0CF01FCE8}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>31</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>341</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>342</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>343</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5E5B8F-5BB7-4168-B07F-5847C1B5455F}">
   <dimension ref="A1:F5"/>
@@ -4181,7 +4452,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>